<commit_message>
updating the GST rates worksheet in SUT file and cess rates excel file
</commit_message>
<xml_diff>
--- a/India Supply Use Table SUT_12-13.xlsx
+++ b/India Supply Use Table SUT_12-13.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb305167\Documents\python\VAT-Gap\VAT-Gap-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49ADFC42-98B6-4D1B-B1CA-83E724CE1F6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7AF895-03E5-44D9-954A-399F55AE10C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8490" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8490" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="supply 2012-13" sheetId="1" r:id="rId1"/>
     <sheet name="use 2012-13" sheetId="9" r:id="rId2"/>
     <sheet name="rates" sheetId="10" r:id="rId3"/>
+    <sheet name="cess_rates" sheetId="11" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'supply 2012-13'!$A$3:$CB$147</definedName>
@@ -107,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="238">
   <si>
     <t>Value in Rs Lakh</t>
   </si>
@@ -819,15 +820,19 @@
   <si>
     <t>srl_no</t>
   </si>
+  <si>
+    <t>cess_rates</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -972,7 +977,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
@@ -989,8 +994,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1034,12 +1040,14 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="15">
     <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma 3" xfId="14" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 12 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
@@ -55993,10 +56001,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D5CBD9-2CA9-455B-B19F-20052C58F7B6}">
-  <dimension ref="A1:C141"/>
+  <dimension ref="A1:D141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56004,9 +56012,10 @@
     <col min="1" max="1" width="6" style="6" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" style="6" customWidth="1"/>
     <col min="3" max="3" width="10.140625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>236</v>
       </c>
@@ -56016,169 +56025,170 @@
       <c r="C1" s="18" t="s">
         <v>234</v>
       </c>
+      <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="19">
+      <c r="C2" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="19">
-        <v>0</v>
+      <c r="C5" s="20">
+        <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="19">
-        <v>0</v>
+      <c r="C11" s="20">
+        <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="19">
-        <v>0</v>
+      <c r="C14" s="20">
+        <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="19">
-        <v>0</v>
+      <c r="C15" s="20">
+        <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="20">
         <v>0</v>
       </c>
     </row>
@@ -56189,7 +56199,7 @@
       <c r="B17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="20">
         <v>0</v>
       </c>
     </row>
@@ -56200,8 +56210,8 @@
       <c r="B18" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="19">
-        <v>0</v>
+      <c r="C18" s="20">
+        <v>0.18</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -56211,7 +56221,7 @@
       <c r="B19" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="20">
         <v>0</v>
       </c>
     </row>
@@ -56222,7 +56232,7 @@
       <c r="B20" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="20">
         <v>0</v>
       </c>
     </row>
@@ -56233,7 +56243,7 @@
       <c r="B21" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="20">
         <v>0</v>
       </c>
     </row>
@@ -56244,7 +56254,7 @@
       <c r="B22" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="20">
         <v>0</v>
       </c>
     </row>
@@ -56255,7 +56265,7 @@
       <c r="B23" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="20">
         <v>0</v>
       </c>
     </row>
@@ -56266,7 +56276,7 @@
       <c r="B24" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="20">
         <v>0</v>
       </c>
     </row>
@@ -56277,8 +56287,8 @@
       <c r="B25" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C25" s="19">
-        <v>0</v>
+      <c r="C25" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -56288,8 +56298,8 @@
       <c r="B26" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C26" s="19">
-        <v>0</v>
+      <c r="C26" s="20">
+        <v>0.12</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -56299,7 +56309,7 @@
       <c r="B27" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C27" s="19">
+      <c r="C27" s="20">
         <v>0</v>
       </c>
     </row>
@@ -56310,8 +56320,8 @@
       <c r="B28" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C28" s="19">
-        <v>0</v>
+      <c r="C28" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -56321,7 +56331,7 @@
       <c r="B29" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C29" s="19">
+      <c r="C29" s="20">
         <v>0</v>
       </c>
     </row>
@@ -56332,7 +56342,7 @@
       <c r="B30" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="20">
         <v>0</v>
       </c>
     </row>
@@ -56343,8 +56353,8 @@
       <c r="B31" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C31" s="19">
-        <v>0</v>
+      <c r="C31" s="20">
+        <v>0.15</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -56354,8 +56364,8 @@
       <c r="B32" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="19">
-        <v>0</v>
+      <c r="C32" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -56365,7 +56375,7 @@
       <c r="B33" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C33" s="19">
+      <c r="C33" s="20">
         <v>0</v>
       </c>
     </row>
@@ -56376,8 +56386,8 @@
       <c r="B34" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C34" s="19">
-        <v>0</v>
+      <c r="C34" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -56387,8 +56397,8 @@
       <c r="B35" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C35" s="19">
-        <v>0</v>
+      <c r="C35" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -56398,8 +56408,8 @@
       <c r="B36" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C36" s="19">
-        <v>0</v>
+      <c r="C36" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -56409,8 +56419,8 @@
       <c r="B37" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C37" s="19">
-        <v>0</v>
+      <c r="C37" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -56420,8 +56430,8 @@
       <c r="B38" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C38" s="19">
-        <v>0</v>
+      <c r="C38" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -56431,8 +56441,8 @@
       <c r="B39" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C39" s="19">
-        <v>0</v>
+      <c r="C39" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -56442,8 +56452,8 @@
       <c r="B40" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C40" s="19">
-        <v>0</v>
+      <c r="C40" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -56453,8 +56463,8 @@
       <c r="B41" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C41" s="19">
-        <v>0</v>
+      <c r="C41" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -56464,8 +56474,8 @@
       <c r="B42" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C42" s="19">
-        <v>0</v>
+      <c r="C42" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -56475,8 +56485,8 @@
       <c r="B43" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C43" s="19">
-        <v>0</v>
+      <c r="C43" s="20">
+        <v>0.12</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -56486,8 +56496,8 @@
       <c r="B44" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C44" s="19">
-        <v>0</v>
+      <c r="C44" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -56497,8 +56507,8 @@
       <c r="B45" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C45" s="19">
-        <v>0</v>
+      <c r="C45" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -56508,8 +56518,8 @@
       <c r="B46" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C46" s="19">
-        <v>0</v>
+      <c r="C46" s="20">
+        <v>0.12</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -56519,8 +56529,8 @@
       <c r="B47" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C47" s="19">
-        <v>0</v>
+      <c r="C47" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -56530,8 +56540,8 @@
       <c r="B48" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C48" s="19">
-        <v>0</v>
+      <c r="C48" s="20">
+        <v>0.12</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -56541,8 +56551,8 @@
       <c r="B49" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C49" s="19">
-        <v>0</v>
+      <c r="C49" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -56552,8 +56562,8 @@
       <c r="B50" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C50" s="19">
-        <v>0</v>
+      <c r="C50" s="20">
+        <v>0.18</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -56563,8 +56573,8 @@
       <c r="B51" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C51" s="19">
-        <v>0</v>
+      <c r="C51" s="20">
+        <v>0.18</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -56574,7 +56584,7 @@
       <c r="B52" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C52" s="19">
+      <c r="C52" s="20">
         <v>0</v>
       </c>
     </row>
@@ -56585,8 +56595,8 @@
       <c r="B53" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C53" s="19">
-        <v>0</v>
+      <c r="C53" s="20">
+        <v>0.18</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -56596,8 +56606,8 @@
       <c r="B54" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C54" s="19">
-        <v>0</v>
+      <c r="C54" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -56607,8 +56617,8 @@
       <c r="B55" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C55" s="19">
-        <v>0</v>
+      <c r="C55" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -56618,8 +56628,8 @@
       <c r="B56" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="C56" s="19">
-        <v>0.18</v>
+      <c r="C56" s="20">
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -56629,8 +56639,8 @@
       <c r="B57" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C57" s="19">
-        <v>0.18</v>
+      <c r="C57" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -56640,8 +56650,8 @@
       <c r="B58" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C58" s="19">
-        <v>0.18</v>
+      <c r="C58" s="20">
+        <v>0.12</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -56651,8 +56661,8 @@
       <c r="B59" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C59" s="19">
-        <v>0.18</v>
+      <c r="C59" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -56662,8 +56672,8 @@
       <c r="B60" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="C60" s="19">
-        <v>0.18</v>
+      <c r="C60" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -56673,8 +56683,8 @@
       <c r="B61" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="C61" s="19">
-        <v>0.18</v>
+      <c r="C61" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -56684,8 +56694,8 @@
       <c r="B62" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="C62" s="19">
-        <v>0.18</v>
+      <c r="C62" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -56695,8 +56705,8 @@
       <c r="B63" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C63" s="19">
-        <v>0.18</v>
+      <c r="C63" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -56706,7 +56716,7 @@
       <c r="B64" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C64" s="19">
+      <c r="C64" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -56717,7 +56727,7 @@
       <c r="B65" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C65" s="19">
+      <c r="C65" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -56728,8 +56738,8 @@
       <c r="B66" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C66" s="19">
-        <v>0.18</v>
+      <c r="C66" s="20">
+        <v>0.12</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -56739,8 +56749,8 @@
       <c r="B67" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C67" s="19">
-        <v>0.18</v>
+      <c r="C67" s="20">
+        <v>0.12</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -56750,7 +56760,7 @@
       <c r="B68" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C68" s="19">
+      <c r="C68" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -56761,7 +56771,7 @@
       <c r="B69" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C69" s="19">
+      <c r="C69" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -56772,7 +56782,7 @@
       <c r="B70" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C70" s="19">
+      <c r="C70" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -56783,7 +56793,7 @@
       <c r="B71" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C71" s="19">
+      <c r="C71" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -56794,8 +56804,8 @@
       <c r="B72" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="C72" s="19">
-        <v>0.18</v>
+      <c r="C72" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -56805,7 +56815,7 @@
       <c r="B73" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="C73" s="19">
+      <c r="C73" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -56816,7 +56826,7 @@
       <c r="B74" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="C74" s="19">
+      <c r="C74" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -56827,7 +56837,7 @@
       <c r="B75" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="C75" s="19">
+      <c r="C75" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -56838,8 +56848,8 @@
       <c r="B76" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="C76" s="19">
-        <v>0.18</v>
+      <c r="C76" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -56849,7 +56859,7 @@
       <c r="B77" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="C77" s="19">
+      <c r="C77" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -56860,7 +56870,7 @@
       <c r="B78" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="C78" s="19">
+      <c r="C78" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -56871,8 +56881,8 @@
       <c r="B79" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="C79" s="19">
-        <v>0.18</v>
+      <c r="C79" s="20">
+        <v>0.12</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -56882,7 +56892,7 @@
       <c r="B80" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="C80" s="19">
+      <c r="C80" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -56893,8 +56903,8 @@
       <c r="B81" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="C81" s="19">
-        <v>0.18</v>
+      <c r="C81" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -56904,7 +56914,7 @@
       <c r="B82" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C82" s="19">
+      <c r="C82" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -56915,8 +56925,8 @@
       <c r="B83" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C83" s="19">
-        <v>0.18</v>
+      <c r="C83" s="20">
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -56926,7 +56936,7 @@
       <c r="B84" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="C84" s="19">
+      <c r="C84" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -56937,7 +56947,7 @@
       <c r="B85" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="C85" s="19">
+      <c r="C85" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -56948,7 +56958,7 @@
       <c r="B86" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="C86" s="19">
+      <c r="C86" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -56959,7 +56969,7 @@
       <c r="B87" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="C87" s="19">
+      <c r="C87" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -56970,7 +56980,7 @@
       <c r="B88" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="C88" s="19">
+      <c r="C88" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -56981,7 +56991,7 @@
       <c r="B89" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="C89" s="19">
+      <c r="C89" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -56992,7 +57002,7 @@
       <c r="B90" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="C90" s="19">
+      <c r="C90" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57003,8 +57013,8 @@
       <c r="B91" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="C91" s="19">
-        <v>0.18</v>
+      <c r="C91" s="20">
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -57014,7 +57024,7 @@
       <c r="B92" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C92" s="19">
+      <c r="C92" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57025,7 +57035,7 @@
       <c r="B93" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="C93" s="19">
+      <c r="C93" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57036,7 +57046,7 @@
       <c r="B94" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="C94" s="19">
+      <c r="C94" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57047,7 +57057,7 @@
       <c r="B95" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="C95" s="19">
+      <c r="C95" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57058,7 +57068,7 @@
       <c r="B96" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="C96" s="19">
+      <c r="C96" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57069,7 +57079,7 @@
       <c r="B97" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C97" s="19">
+      <c r="C97" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57080,8 +57090,8 @@
       <c r="B98" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C98" s="19">
-        <v>0.18</v>
+      <c r="C98" s="20">
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -57091,8 +57101,8 @@
       <c r="B99" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="C99" s="19">
-        <v>0.18</v>
+      <c r="C99" s="20">
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -57102,8 +57112,8 @@
       <c r="B100" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C100" s="19">
-        <v>0.18</v>
+      <c r="C100" s="20">
+        <v>0.12</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -57113,8 +57123,8 @@
       <c r="B101" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="C101" s="19">
-        <v>0.18</v>
+      <c r="C101" s="20">
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -57124,8 +57134,8 @@
       <c r="B102" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C102" s="19">
-        <v>0.18</v>
+      <c r="C102" s="20">
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -57135,8 +57145,8 @@
       <c r="B103" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="C103" s="19">
-        <v>0.18</v>
+      <c r="C103" s="20">
+        <v>0.12</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -57146,7 +57156,7 @@
       <c r="B104" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="C104" s="19">
+      <c r="C104" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57157,8 +57167,8 @@
       <c r="B105" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="C105" s="19">
-        <v>0.18</v>
+      <c r="C105" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -57168,8 +57178,8 @@
       <c r="B106" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="C106" s="19">
-        <v>0.18</v>
+      <c r="C106" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -57179,8 +57189,8 @@
       <c r="B107" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="C107" s="19">
-        <v>0.18</v>
+      <c r="C107" s="20">
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -57190,8 +57200,8 @@
       <c r="B108" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="C108" s="19">
-        <v>0.18</v>
+      <c r="C108" s="20">
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -57201,8 +57211,8 @@
       <c r="B109" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="C109" s="19">
-        <v>0.18</v>
+      <c r="C109" s="20">
+        <v>0.12</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -57212,8 +57222,8 @@
       <c r="B110" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C110" s="19">
-        <v>0.18</v>
+      <c r="C110" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -57223,7 +57233,7 @@
       <c r="B111" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="C111" s="19">
+      <c r="C111" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57234,8 +57244,8 @@
       <c r="B112" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C112" s="19">
-        <v>0.18</v>
+      <c r="C112" s="20">
+        <v>0.03</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -57245,7 +57255,7 @@
       <c r="B113" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="C113" s="19">
+      <c r="C113" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57256,7 +57266,7 @@
       <c r="B114" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="C114" s="19">
+      <c r="C114" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57267,8 +57277,8 @@
       <c r="B115" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C115" s="19">
-        <v>0.18</v>
+      <c r="C115" s="20">
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -57278,8 +57288,8 @@
       <c r="B116" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C116" s="19">
-        <v>0.18</v>
+      <c r="C116" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -57289,8 +57299,8 @@
       <c r="B117" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="C117" s="19">
-        <v>0.18</v>
+      <c r="C117" s="20">
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -57300,7 +57310,7 @@
       <c r="B118" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C118" s="19">
+      <c r="C118" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57311,7 +57321,7 @@
       <c r="B119" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="C119" s="19">
+      <c r="C119" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57322,8 +57332,8 @@
       <c r="B120" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C120" s="19">
-        <v>0.18</v>
+      <c r="C120" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -57333,8 +57343,8 @@
       <c r="B121" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C121" s="19">
-        <v>0.18</v>
+      <c r="C121" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -57344,8 +57354,8 @@
       <c r="B122" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="C122" s="19">
-        <v>0.18</v>
+      <c r="C122" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -57355,8 +57365,8 @@
       <c r="B123" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C123" s="19">
-        <v>0.18</v>
+      <c r="C123" s="20">
+        <v>0.05</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -57366,7 +57376,7 @@
       <c r="B124" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C124" s="19">
+      <c r="C124" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57377,7 +57387,7 @@
       <c r="B125" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C125" s="19">
+      <c r="C125" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57388,7 +57398,7 @@
       <c r="B126" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="C126" s="19">
+      <c r="C126" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57399,7 +57409,7 @@
       <c r="B127" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C127" s="19">
+      <c r="C127" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57410,7 +57420,7 @@
       <c r="B128" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="C128" s="19">
+      <c r="C128" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57421,7 +57431,7 @@
       <c r="B129" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="C129" s="19">
+      <c r="C129" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57432,7 +57442,7 @@
       <c r="B130" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="C130" s="19">
+      <c r="C130" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57443,7 +57453,7 @@
       <c r="B131" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="C131" s="19">
+      <c r="C131" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57454,7 +57464,7 @@
       <c r="B132" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="C132" s="19">
+      <c r="C132" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57465,7 +57475,7 @@
       <c r="B133" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="C133" s="19">
+      <c r="C133" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57476,7 +57486,7 @@
       <c r="B134" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="C134" s="19">
+      <c r="C134" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57487,7 +57497,7 @@
       <c r="B135" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C135" s="19">
+      <c r="C135" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57498,7 +57508,7 @@
       <c r="B136" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C136" s="19">
+      <c r="C136" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57509,7 +57519,7 @@
       <c r="B137" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="C137" s="19">
+      <c r="C137" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57520,7 +57530,7 @@
       <c r="B138" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="C138" s="19">
+      <c r="C138" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57531,7 +57541,7 @@
       <c r="B139" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="C139" s="19">
+      <c r="C139" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57542,7 +57552,7 @@
       <c r="B140" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="C140" s="19">
+      <c r="C140" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57553,7 +57563,7 @@
       <c r="B141" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="C141" s="19">
+      <c r="C141" s="20">
         <v>0.18</v>
       </c>
     </row>
@@ -57561,4 +57571,1573 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9294B521-AC8C-436A-A976-E4547F3227D2}">
+  <dimension ref="A1:C141"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6" style="21" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="21" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
+        <v>2</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
+        <v>3</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
+        <v>4</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="21">
+        <v>5</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
+        <v>6</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="21">
+        <v>7</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="21">
+        <v>8</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="21">
+        <v>9</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
+        <v>10</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="21">
+        <v>11</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="21">
+        <v>12</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="21">
+        <v>13</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="21">
+        <v>14</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="21">
+        <v>15</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
+        <v>16</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="21">
+        <v>17</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="21">
+        <v>18</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="21">
+        <v>19</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="21">
+        <v>21</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="21">
+        <v>22</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="21">
+        <v>23</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="21">
+        <v>24</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="21">
+        <v>25</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="21">
+        <v>26</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="21">
+        <v>27</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="21">
+        <v>28</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="21">
+        <v>29</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="21">
+        <v>30</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="21">
+        <v>31</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="21">
+        <v>32</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="21">
+        <v>33</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="21">
+        <v>34</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="21">
+        <v>35</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="21">
+        <v>36</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="21">
+        <v>37</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="21">
+        <v>38</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="21">
+        <v>39</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="21">
+        <v>40</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="21">
+        <v>41</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="21">
+        <v>42</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="21">
+        <v>43</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="21">
+        <v>44</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C45" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="21">
+        <v>45</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="21">
+        <v>46</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C47" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="21">
+        <v>47</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C48" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="21">
+        <v>48</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="C49" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="21">
+        <v>49</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="C50" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="21">
+        <v>50</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C51" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="21">
+        <v>51</v>
+      </c>
+      <c r="B52" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="21">
+        <v>52</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="21">
+        <v>53</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="21">
+        <v>54</v>
+      </c>
+      <c r="B55" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="C55" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="21">
+        <v>55</v>
+      </c>
+      <c r="B56" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C56" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="21">
+        <v>56</v>
+      </c>
+      <c r="B57" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="C57" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="21">
+        <v>57</v>
+      </c>
+      <c r="B58" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="C58" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="21">
+        <v>58</v>
+      </c>
+      <c r="B59" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C59" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="21">
+        <v>59</v>
+      </c>
+      <c r="B60" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="C60" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="21">
+        <v>60</v>
+      </c>
+      <c r="B61" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C61" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="21">
+        <v>61</v>
+      </c>
+      <c r="B62" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="C62" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="21">
+        <v>62</v>
+      </c>
+      <c r="B63" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="C63" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="21">
+        <v>63</v>
+      </c>
+      <c r="B64" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="C64" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="21">
+        <v>64</v>
+      </c>
+      <c r="B65" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C65" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="21">
+        <v>65</v>
+      </c>
+      <c r="B66" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="C66" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="21">
+        <v>66</v>
+      </c>
+      <c r="B67" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="C67" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="21">
+        <v>67</v>
+      </c>
+      <c r="B68" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="C68" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="21">
+        <v>68</v>
+      </c>
+      <c r="B69" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C69" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="21">
+        <v>69</v>
+      </c>
+      <c r="B70" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="C70" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="21">
+        <v>70</v>
+      </c>
+      <c r="B71" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="C71" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="21">
+        <v>71</v>
+      </c>
+      <c r="B72" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C72" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="21">
+        <v>72</v>
+      </c>
+      <c r="B73" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="C73" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="21">
+        <v>73</v>
+      </c>
+      <c r="B74" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="C74" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="21">
+        <v>74</v>
+      </c>
+      <c r="B75" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="C75" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="21">
+        <v>75</v>
+      </c>
+      <c r="B76" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C76" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="21">
+        <v>76</v>
+      </c>
+      <c r="B77" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="C77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="21">
+        <v>77</v>
+      </c>
+      <c r="B78" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="C78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="21">
+        <v>78</v>
+      </c>
+      <c r="B79" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="C79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="21">
+        <v>79</v>
+      </c>
+      <c r="B80" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="C80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="21">
+        <v>80</v>
+      </c>
+      <c r="B81" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="C81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="21">
+        <v>81</v>
+      </c>
+      <c r="B82" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="C82" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="21">
+        <v>82</v>
+      </c>
+      <c r="B83" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="C83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="21">
+        <v>83</v>
+      </c>
+      <c r="B84" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="21">
+        <v>84</v>
+      </c>
+      <c r="B85" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="C85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="21">
+        <v>85</v>
+      </c>
+      <c r="B86" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C86" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="21">
+        <v>86</v>
+      </c>
+      <c r="B87" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="C87" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="21">
+        <v>87</v>
+      </c>
+      <c r="B88" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="C88" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="21">
+        <v>88</v>
+      </c>
+      <c r="B89" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C89" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="21">
+        <v>89</v>
+      </c>
+      <c r="B90" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="21">
+        <v>90</v>
+      </c>
+      <c r="B91" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="C91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="21">
+        <v>91</v>
+      </c>
+      <c r="B92" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="C92" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="21">
+        <v>92</v>
+      </c>
+      <c r="B93" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="C93" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="21">
+        <v>93</v>
+      </c>
+      <c r="B94" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="C94" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="21">
+        <v>94</v>
+      </c>
+      <c r="B95" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C95" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="21">
+        <v>95</v>
+      </c>
+      <c r="B96" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="C96" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="21">
+        <v>96</v>
+      </c>
+      <c r="B97" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="C97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="21">
+        <v>97</v>
+      </c>
+      <c r="B98" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="C98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="21">
+        <v>98</v>
+      </c>
+      <c r="B99" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="C99" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="21">
+        <v>99</v>
+      </c>
+      <c r="B100" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="21">
+        <v>100</v>
+      </c>
+      <c r="B101" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="C101" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="21">
+        <v>101</v>
+      </c>
+      <c r="B102" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="C102" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="21">
+        <v>102</v>
+      </c>
+      <c r="B103" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="C103" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="21">
+        <v>103</v>
+      </c>
+      <c r="B104" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="C104" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="21">
+        <v>104</v>
+      </c>
+      <c r="B105" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="C105" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="21">
+        <v>105</v>
+      </c>
+      <c r="B106" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="C106" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="21">
+        <v>106</v>
+      </c>
+      <c r="B107" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="C107" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="21">
+        <v>107</v>
+      </c>
+      <c r="B108" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="C108" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="21">
+        <v>108</v>
+      </c>
+      <c r="B109" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="C109" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="21">
+        <v>109</v>
+      </c>
+      <c r="B110" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="C110" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="21">
+        <v>110</v>
+      </c>
+      <c r="B111" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="C111" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="21">
+        <v>111</v>
+      </c>
+      <c r="B112" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="C112" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="21">
+        <v>112</v>
+      </c>
+      <c r="B113" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="C113" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="21">
+        <v>113</v>
+      </c>
+      <c r="B114" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="C114" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="21">
+        <v>114</v>
+      </c>
+      <c r="B115" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C115" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="21">
+        <v>115</v>
+      </c>
+      <c r="B116" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C116" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="21">
+        <v>116</v>
+      </c>
+      <c r="B117" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="C117" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="21">
+        <v>117</v>
+      </c>
+      <c r="B118" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C118" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="21">
+        <v>118</v>
+      </c>
+      <c r="B119" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="C119" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="21">
+        <v>119</v>
+      </c>
+      <c r="B120" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C120" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="21">
+        <v>120</v>
+      </c>
+      <c r="B121" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C121" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="21">
+        <v>121</v>
+      </c>
+      <c r="B122" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="C122" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="21">
+        <v>122</v>
+      </c>
+      <c r="B123" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="C123" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="21">
+        <v>123</v>
+      </c>
+      <c r="B124" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C124" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="21">
+        <v>124</v>
+      </c>
+      <c r="B125" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="C125" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="21">
+        <v>125</v>
+      </c>
+      <c r="B126" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="C126" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="21">
+        <v>126</v>
+      </c>
+      <c r="B127" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="C127" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="21">
+        <v>127</v>
+      </c>
+      <c r="B128" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="C128" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="21">
+        <v>128</v>
+      </c>
+      <c r="B129" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="C129" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="21">
+        <v>129</v>
+      </c>
+      <c r="B130" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="C130" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="21">
+        <v>130</v>
+      </c>
+      <c r="B131" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="C131" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="21">
+        <v>131</v>
+      </c>
+      <c r="B132" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="C132" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="21">
+        <v>132</v>
+      </c>
+      <c r="B133" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="C133" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="21">
+        <v>133</v>
+      </c>
+      <c r="B134" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="C134" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="21">
+        <v>134</v>
+      </c>
+      <c r="B135" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C135" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="21">
+        <v>135</v>
+      </c>
+      <c r="B136" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C136" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="21">
+        <v>136</v>
+      </c>
+      <c r="B137" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="C137" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="21">
+        <v>137</v>
+      </c>
+      <c r="B138" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="C138" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="21">
+        <v>138</v>
+      </c>
+      <c r="B139" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="C139" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="21">
+        <v>139</v>
+      </c>
+      <c r="B140" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="C140" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="21">
+        <v>140</v>
+      </c>
+      <c r="B141" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="C141" s="22">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding the exempt ratiop and ITC disallowance
</commit_message>
<xml_diff>
--- a/India Supply Use Table SUT_12-13.xlsx
+++ b/India Supply Use Table SUT_12-13.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb305167\Documents\python\VAT-Gap\VAT-Gap-Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\VAT GAP\VAT-Gap-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7AF895-03E5-44D9-954A-399F55AE10C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8490" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8490" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="supply 2012-13" sheetId="1" r:id="rId1"/>
     <sheet name="use 2012-13" sheetId="9" r:id="rId2"/>
     <sheet name="rates" sheetId="10" r:id="rId3"/>
     <sheet name="cess_rates" sheetId="11" r:id="rId4"/>
+    <sheet name="exempt" sheetId="12" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'supply 2012-13'!$A$3:$CB$147</definedName>
@@ -28,7 +28,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'supply 2012-13'!$A:$B,'supply 2012-13'!$1:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'use 2012-13'!$A:$B,'use 2012-13'!$1:$3</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,12 +40,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Lenovo</author>
   </authors>
   <commentList>
-    <comment ref="BT97" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="BT97" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -74,12 +74,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Lenovo</author>
   </authors>
   <commentList>
-    <comment ref="BW114" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="BW114" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="239">
   <si>
     <t>Value in Rs Lakh</t>
   </si>
@@ -823,16 +823,19 @@
   <si>
     <t>cess_rates</t>
   </si>
+  <si>
+    <t>exempt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0_)"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -979,7 +982,7 @@
   </borders>
   <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
@@ -987,16 +990,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1008,7 +1011,7 @@
     <xf numFmtId="1" fontId="11" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1020,10 +1023,10 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1044,23 +1047,29 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="15">
-    <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Comma 3" xfId="14" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Comma 2" xfId="1"/>
+    <cellStyle name="Comma 3" xfId="14"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 12 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal 2 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal 3 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal 4" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Normal 4 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Normal 5" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal 5 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Percent 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="s73" xfId="13" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 12 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 2 2" xfId="4"/>
+    <cellStyle name="Normal 2 3" xfId="5"/>
+    <cellStyle name="Normal 3" xfId="6"/>
+    <cellStyle name="Normal 3 2" xfId="7"/>
+    <cellStyle name="Normal 4" xfId="8"/>
+    <cellStyle name="Normal 4 2" xfId="9"/>
+    <cellStyle name="Normal 5" xfId="10"/>
+    <cellStyle name="Normal 5 2" xfId="11"/>
+    <cellStyle name="Percent 2" xfId="12"/>
+    <cellStyle name="s73" xfId="13"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1151,23 +1160,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1203,23 +1195,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1395,15 +1370,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CE145"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C37" activePane="bottomRight" state="frozen"/>
       <selection activeCell="BQ149" sqref="BQ149"/>
       <selection pane="topRight" activeCell="BQ149" sqref="BQ149"/>
       <selection pane="bottomLeft" activeCell="BQ149" sqref="BQ149"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="A51" sqref="A51:XFD51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22081,7 +22056,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:CB147" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A3:CB147"/>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.27559055118110237" bottom="0.23622047244094491" header="0.31496062992125984" footer="0.23622047244094491"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -22089,11 +22064,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CB152"/>
   <sheetViews>
     <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="BN4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="BQ149" sqref="BQ149"/>
       <selection pane="topRight" activeCell="BQ149" sqref="BQ149"/>
       <selection pane="bottomLeft" activeCell="BQ149" sqref="BQ149"/>
@@ -55992,7 +55967,7 @@
       <c r="BY152" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:BY146" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A3:BY146"/>
   <pageMargins left="0.17" right="0.17" top="0.24" bottom="0.24" header="0.31496062992125984" footer="0.24"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -56000,7 +55975,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D5CBD9-2CA9-455B-B19F-20052C58F7B6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -57574,10 +57549,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9294B521-AC8C-436A-A976-E4547F3227D2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -59140,4 +59115,1575 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C141"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6" style="21" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="21" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
+        <v>2</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
+        <v>3</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
+        <v>4</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="21">
+        <v>5</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
+        <v>6</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="21">
+        <v>7</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="21">
+        <v>8</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="21">
+        <v>9</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
+        <v>10</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="21">
+        <v>11</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="21">
+        <v>12</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="21">
+        <v>13</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="21">
+        <v>14</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="21">
+        <v>15</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
+        <v>16</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="21">
+        <v>17</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="21">
+        <v>18</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="21">
+        <v>19</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="21">
+        <v>21</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="21">
+        <v>22</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="21">
+        <v>23</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="21">
+        <v>24</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="21">
+        <v>25</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="21">
+        <v>26</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="21">
+        <v>27</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="21">
+        <v>28</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="21">
+        <v>29</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="21">
+        <v>30</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="21">
+        <v>31</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="21">
+        <v>32</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="21">
+        <v>33</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="21">
+        <v>34</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="21">
+        <v>35</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="21">
+        <v>36</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="21">
+        <v>37</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="21">
+        <v>38</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="21">
+        <v>39</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="21">
+        <v>40</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="21">
+        <v>41</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="21">
+        <v>42</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="21">
+        <v>43</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="21">
+        <v>44</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C45" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="21">
+        <v>45</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="21">
+        <v>46</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C47" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="21">
+        <v>47</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C48" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="21">
+        <v>48</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="C49" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="21">
+        <v>49</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="C50" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="21">
+        <v>50</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C51" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="21">
+        <v>51</v>
+      </c>
+      <c r="B52" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="21">
+        <v>52</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="21">
+        <v>53</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="21">
+        <v>54</v>
+      </c>
+      <c r="B55" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="C55" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="21">
+        <v>55</v>
+      </c>
+      <c r="B56" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C56" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="21">
+        <v>56</v>
+      </c>
+      <c r="B57" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="C57" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="21">
+        <v>57</v>
+      </c>
+      <c r="B58" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="C58" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="21">
+        <v>58</v>
+      </c>
+      <c r="B59" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C59" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="21">
+        <v>59</v>
+      </c>
+      <c r="B60" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="C60" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="21">
+        <v>60</v>
+      </c>
+      <c r="B61" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C61" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="21">
+        <v>61</v>
+      </c>
+      <c r="B62" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="C62" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="21">
+        <v>62</v>
+      </c>
+      <c r="B63" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="C63" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="21">
+        <v>63</v>
+      </c>
+      <c r="B64" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="C64" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="21">
+        <v>64</v>
+      </c>
+      <c r="B65" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C65" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="21">
+        <v>65</v>
+      </c>
+      <c r="B66" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="C66" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="21">
+        <v>66</v>
+      </c>
+      <c r="B67" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="C67" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="21">
+        <v>67</v>
+      </c>
+      <c r="B68" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="C68" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="21">
+        <v>68</v>
+      </c>
+      <c r="B69" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C69" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="21">
+        <v>69</v>
+      </c>
+      <c r="B70" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="C70" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="21">
+        <v>70</v>
+      </c>
+      <c r="B71" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="C71" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="21">
+        <v>71</v>
+      </c>
+      <c r="B72" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C72" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="21">
+        <v>72</v>
+      </c>
+      <c r="B73" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="C73" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="21">
+        <v>73</v>
+      </c>
+      <c r="B74" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="C74" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="21">
+        <v>74</v>
+      </c>
+      <c r="B75" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="C75" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="21">
+        <v>75</v>
+      </c>
+      <c r="B76" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C76" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="21">
+        <v>76</v>
+      </c>
+      <c r="B77" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="C77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="21">
+        <v>77</v>
+      </c>
+      <c r="B78" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="C78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="21">
+        <v>78</v>
+      </c>
+      <c r="B79" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="C79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="21">
+        <v>79</v>
+      </c>
+      <c r="B80" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="C80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="21">
+        <v>80</v>
+      </c>
+      <c r="B81" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="C81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="21">
+        <v>81</v>
+      </c>
+      <c r="B82" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="C82" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="21">
+        <v>82</v>
+      </c>
+      <c r="B83" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="C83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="21">
+        <v>83</v>
+      </c>
+      <c r="B84" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="21">
+        <v>84</v>
+      </c>
+      <c r="B85" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="C85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="21">
+        <v>85</v>
+      </c>
+      <c r="B86" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C86" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="21">
+        <v>86</v>
+      </c>
+      <c r="B87" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="C87" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="21">
+        <v>87</v>
+      </c>
+      <c r="B88" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="C88" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="21">
+        <v>88</v>
+      </c>
+      <c r="B89" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C89" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="21">
+        <v>89</v>
+      </c>
+      <c r="B90" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="21">
+        <v>90</v>
+      </c>
+      <c r="B91" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="C91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="21">
+        <v>91</v>
+      </c>
+      <c r="B92" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="C92" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="21">
+        <v>92</v>
+      </c>
+      <c r="B93" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="C93" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="21">
+        <v>93</v>
+      </c>
+      <c r="B94" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="C94" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="21">
+        <v>94</v>
+      </c>
+      <c r="B95" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C95" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="21">
+        <v>95</v>
+      </c>
+      <c r="B96" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="C96" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="21">
+        <v>96</v>
+      </c>
+      <c r="B97" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="C97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="21">
+        <v>97</v>
+      </c>
+      <c r="B98" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="C98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="21">
+        <v>98</v>
+      </c>
+      <c r="B99" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="C99" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="21">
+        <v>99</v>
+      </c>
+      <c r="B100" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="21">
+        <v>100</v>
+      </c>
+      <c r="B101" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="C101" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="21">
+        <v>101</v>
+      </c>
+      <c r="B102" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="C102" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="21">
+        <v>102</v>
+      </c>
+      <c r="B103" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="C103" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="21">
+        <v>103</v>
+      </c>
+      <c r="B104" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="C104" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="21">
+        <v>104</v>
+      </c>
+      <c r="B105" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="C105" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="21">
+        <v>105</v>
+      </c>
+      <c r="B106" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="C106" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="21">
+        <v>106</v>
+      </c>
+      <c r="B107" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="C107" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="21">
+        <v>107</v>
+      </c>
+      <c r="B108" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="C108" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="21">
+        <v>108</v>
+      </c>
+      <c r="B109" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="C109" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="21">
+        <v>109</v>
+      </c>
+      <c r="B110" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="C110" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="21">
+        <v>110</v>
+      </c>
+      <c r="B111" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="C111" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="21">
+        <v>111</v>
+      </c>
+      <c r="B112" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="C112" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="21">
+        <v>112</v>
+      </c>
+      <c r="B113" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="C113" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="21">
+        <v>113</v>
+      </c>
+      <c r="B114" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="C114" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="21">
+        <v>114</v>
+      </c>
+      <c r="B115" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C115" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="21">
+        <v>115</v>
+      </c>
+      <c r="B116" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C116" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="21">
+        <v>116</v>
+      </c>
+      <c r="B117" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="C117" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="21">
+        <v>117</v>
+      </c>
+      <c r="B118" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C118" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="21">
+        <v>118</v>
+      </c>
+      <c r="B119" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="C119" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="21">
+        <v>119</v>
+      </c>
+      <c r="B120" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C120" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="21">
+        <v>120</v>
+      </c>
+      <c r="B121" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C121" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="21">
+        <v>121</v>
+      </c>
+      <c r="B122" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="C122" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="21">
+        <v>122</v>
+      </c>
+      <c r="B123" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="C123" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="21">
+        <v>123</v>
+      </c>
+      <c r="B124" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C124" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="21">
+        <v>124</v>
+      </c>
+      <c r="B125" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="C125" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="21">
+        <v>125</v>
+      </c>
+      <c r="B126" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="C126" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="21">
+        <v>126</v>
+      </c>
+      <c r="B127" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="C127" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="21">
+        <v>127</v>
+      </c>
+      <c r="B128" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="C128" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="21">
+        <v>128</v>
+      </c>
+      <c r="B129" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="C129" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="21">
+        <v>129</v>
+      </c>
+      <c r="B130" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="C130" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="21">
+        <v>130</v>
+      </c>
+      <c r="B131" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="C131" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="21">
+        <v>131</v>
+      </c>
+      <c r="B132" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="C132" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="21">
+        <v>132</v>
+      </c>
+      <c r="B133" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="C133" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="21">
+        <v>133</v>
+      </c>
+      <c r="B134" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="C134" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="21">
+        <v>134</v>
+      </c>
+      <c r="B135" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C135" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="21">
+        <v>135</v>
+      </c>
+      <c r="B136" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C136" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="21">
+        <v>136</v>
+      </c>
+      <c r="B137" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="C137" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="21">
+        <v>137</v>
+      </c>
+      <c r="B138" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="C138" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="21">
+        <v>138</v>
+      </c>
+      <c r="B139" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="C139" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="21">
+        <v>139</v>
+      </c>
+      <c r="B140" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="C140" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="21">
+        <v>140</v>
+      </c>
+      <c r="B141" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="C141" s="22">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>